<commit_message>
Update trends to be calculated over short time frame
</commit_message>
<xml_diff>
--- a/Output/Difference in moving averages16Oct.xlsx
+++ b/Output/Difference in moving averages16Oct.xlsx
@@ -382,12 +382,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>31-day average of new cases per million</t>
+          <t>31-day average of new cases per million on end_date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>61-day average of new cases per million</t>
+          <t>61-day average of new cases per million on end_date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -427,7 +427,7 @@
         <v>1.04227868852459</v>
       </c>
       <c r="F2">
-        <v>0.5872416467177437</v>
+        <v>0.6646505787510942</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -461,7 +461,7 @@
         <v>5.848393442622951</v>
       </c>
       <c r="F3">
-        <v>0.2985269266792627</v>
+        <v>0.4683578650224575</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -495,7 +495,7 @@
         <v>2.491</v>
       </c>
       <c r="F4">
-        <v>0.05434452625953953</v>
+        <v>0.04717198440667601</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -529,7 +529,7 @@
         <v>10.95295081967213</v>
       </c>
       <c r="F5">
-        <v>0.7993996248999115</v>
+        <v>0.8020266219923539</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
         <v>0.5855245901639344</v>
       </c>
       <c r="F6">
-        <v>0.1080218633798786</v>
+        <v>0.1269449380071233</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -597,7 +597,7 @@
         <v>3.888</v>
       </c>
       <c r="F7">
-        <v>0.1400844854531578</v>
+        <v>0.1514945877505779</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>56.41845901639344</v>
       </c>
       <c r="F8">
-        <v>4.723557627702017</v>
+        <v>5.231632067231535</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -665,7 +665,7 @@
         <v>0.8516557377049181</v>
       </c>
       <c r="F9">
-        <v>0.03887609079649619</v>
+        <v>0.03769593259332928</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -699,7 +699,7 @@
         <v>0.1612459016393443</v>
       </c>
       <c r="F10">
-        <v>0.02273825606395596</v>
+        <v>0.02576761226282361</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -733,7 +733,7 @@
         <v>0.009836065573770491</v>
       </c>
       <c r="F11">
-        <v>0.007559121026115737</v>
+        <v>0.0105117177807478</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -767,7 +767,7 @@
         <v>1.835377049180328</v>
       </c>
       <c r="F12">
-        <v>0.3636197570005795</v>
+        <v>0.3423210439033681</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -801,7 +801,7 @@
         <v>126.2263114754098</v>
       </c>
       <c r="F13">
-        <v>1.344924550813918</v>
+        <v>1.19643753588726</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
         <v>0.6890163934426229</v>
       </c>
       <c r="F14">
-        <v>0.817701579872638</v>
+        <v>0.8833403842787558</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
         <v>0.3973114754098361</v>
       </c>
       <c r="F15">
-        <v>0.05257215849532303</v>
+        <v>0.05238726726713257</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         <v>4.191852459016394</v>
       </c>
       <c r="F17">
-        <v>0.3853085010067133</v>
+        <v>0.4802058222636689</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         <v>2.028508196721312</v>
       </c>
       <c r="F18">
-        <v>0.3833535192595218</v>
+        <v>0.447937895704188</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         <v>0.2437377049180328</v>
       </c>
       <c r="F19">
-        <v>0.06156841788533235</v>
+        <v>0.05957478470628003</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
         <v>1.260918032786885</v>
       </c>
       <c r="F20">
-        <v>3.910213123006565</v>
+        <v>3.540284968303395</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1073,7 +1073,7 @@
         <v>1.393229508196721</v>
       </c>
       <c r="F21">
-        <v>0.5075447686629873</v>
+        <v>0.6544366865175697</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
         <v>21.33659016393442</v>
       </c>
       <c r="F22">
-        <v>1.977564383123756</v>
+        <v>2.446938567837631</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1141,7 +1141,7 @@
         <v>0.596344262295082</v>
       </c>
       <c r="F23">
-        <v>0.05715853121371701</v>
+        <v>0.07026389679910525</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1175,7 +1175,7 @@
         <v>8.309786885245902</v>
       </c>
       <c r="F24">
-        <v>0.2658052442876666</v>
+        <v>0.2782680759682457</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         <v>13.26170491803279</v>
       </c>
       <c r="F25">
-        <v>1.134091509815704</v>
+        <v>1.385943623853681</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1243,7 +1243,7 @@
         <v>2.61844262295082</v>
       </c>
       <c r="F26">
-        <v>0.7560144860810816</v>
+        <v>0.8727532659728571</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1277,7 +1277,7 @@
         <v>3.635049180327869</v>
       </c>
       <c r="F27">
-        <v>0.2130335752302872</v>
+        <v>0.1103406614627537</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1311,7 +1311,7 @@
         <v>2.23244262295082</v>
       </c>
       <c r="F28">
-        <v>0.6734276721833681</v>
+        <v>0.4565065171700148</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1345,7 +1345,7 @@
         <v>1.572819672131148</v>
       </c>
       <c r="F29">
-        <v>0.5285890420730578</v>
+        <v>0.5597305662458437</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1379,7 +1379,7 @@
         <v>59.76685245901639</v>
       </c>
       <c r="F30">
-        <v>1.89440371639457</v>
+        <v>2.393757439356828</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
         <v>56.79218032786886</v>
       </c>
       <c r="F31">
-        <v>1.363285604279432</v>
+        <v>0.8392335354877263</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>4.052967213114754</v>
       </c>
       <c r="F32">
-        <v>0.3999120666967139</v>
+        <v>0.441530764366967</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1481,7 +1481,7 @@
         <v>23.02652459016393</v>
       </c>
       <c r="F33">
-        <v>6.078541564138308</v>
+        <v>7.590288217990578</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>0.006754098360655738</v>
       </c>
       <c r="F34">
-        <v>0.00541071586066477</v>
+        <v>0.001370605970829375</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Uncertain</t>
+          <t>Decreasing</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
         <v>0.3792786885245902</v>
       </c>
       <c r="F36">
-        <v>0.1507251297666319</v>
+        <v>0.1623236413003281</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1617,7 +1617,7 @@
         <v>1.793754098360656</v>
       </c>
       <c r="F37">
-        <v>0.3917000208013892</v>
+        <v>0.4841607398356109</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1685,7 +1685,7 @@
         <v>0.6104262295081967</v>
       </c>
       <c r="F39">
-        <v>0.06255865042105857</v>
+        <v>0.04881501539185885</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1719,7 +1719,7 @@
         <v>3.324754098360656</v>
       </c>
       <c r="F40">
-        <v>1.151135326212689</v>
+        <v>1.362676272649147</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
         <v>142.929868852459</v>
       </c>
       <c r="F41">
-        <v>1.467607784227286</v>
+        <v>1.766255866850484</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1787,7 +1787,7 @@
         <v>0.11</v>
       </c>
       <c r="F42">
-        <v>0.05546430431060089</v>
+        <v>0.05205618712337947</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1821,7 +1821,7 @@
         <v>54.4662131147541</v>
       </c>
       <c r="F43">
-        <v>1.353124317042438</v>
+        <v>1.304461570022105</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
         <v>4.062737704918033</v>
       </c>
       <c r="F44">
-        <v>0.1078689466452058</v>
+        <v>0.1068795762173563</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1889,7 +1889,7 @@
         <v>9.634508196721312</v>
       </c>
       <c r="F45">
-        <v>0.4419231044216779</v>
+        <v>0.4574030832463262</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -1923,7 +1923,7 @@
         <v>53.8588524590164</v>
       </c>
       <c r="F46">
-        <v>1.243257445297912</v>
+        <v>1.343573772443284</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         <v>3.063622950819672</v>
       </c>
       <c r="F47">
-        <v>0.3600267861145832</v>
+        <v>0.3994333840854735</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>0.02844262295081967</v>
       </c>
       <c r="F48">
-        <v>0.02935716277874447</v>
+        <v>0.01835022575642796</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2025,7 +2025,7 @@
         <v>0.9593770491803279</v>
       </c>
       <c r="F49">
-        <v>0.08932668211409132</v>
+        <v>0.1220891655420356</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2059,7 +2059,7 @@
         <v>2.460918032786885</v>
       </c>
       <c r="F50">
-        <v>0.7100783079059018</v>
+        <v>0.9037699077885014</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2093,7 +2093,7 @@
         <v>115.3231639344262</v>
       </c>
       <c r="F51">
-        <v>2.757708600965888</v>
+        <v>2.07516037307076</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2127,7 +2127,7 @@
         <v>0.5625573770491803</v>
       </c>
       <c r="F52">
-        <v>0.0472746595035505</v>
+        <v>0.05723161316159362</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2161,7 +2161,7 @@
         <v>28.54090163934426</v>
       </c>
       <c r="F53">
-        <v>0.8084231553124004</v>
+        <v>0.8316127199996822</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2195,7 +2195,7 @@
         <v>3.292049180327869</v>
       </c>
       <c r="F54">
-        <v>0.1521062577774182</v>
+        <v>0.190635994330201</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2229,7 +2229,7 @@
         <v>3.29127868852459</v>
       </c>
       <c r="F55">
-        <v>2.834024090209819</v>
+        <v>2.306458265279454</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>3.246557377049181</v>
       </c>
       <c r="F56">
-        <v>0.2781287021688996</v>
+        <v>0.247298791847078</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
         <v>0.7583442622950819</v>
       </c>
       <c r="F57">
-        <v>0.1322820380256849</v>
+        <v>0.101737136301814</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
         <v>0.6271639344262295</v>
       </c>
       <c r="F59">
-        <v>0.1329227413011573</v>
+        <v>0.09135747490524741</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2396,7 +2396,7 @@
         <v>0.4671475409836066</v>
       </c>
       <c r="F60">
-        <v>0.18483917219311</v>
+        <v>0.1785407038479069</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2430,7 +2430,7 @@
         <v>1.802147540983607</v>
       </c>
       <c r="F61">
-        <v>0.06010184937814645</v>
+        <v>0.08127529438419202</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2464,7 +2464,7 @@
         <v>0.5147868852459017</v>
       </c>
       <c r="F62">
-        <v>0.1760815008477116</v>
+        <v>0.1522415865424555</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2498,7 +2498,7 @@
         <v>28.09096721311476</v>
       </c>
       <c r="F63">
-        <v>1.875549970228211</v>
+        <v>2.382538722946213</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2532,7 +2532,7 @@
         <v>3.126819672131147</v>
       </c>
       <c r="F64">
-        <v>0.1004863192467206</v>
+        <v>0.1065247101826628</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2600,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0.009461510164979359</v>
+        <v>0.009506987478454621</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2634,7 +2634,7 @@
         <v>0.04970491803278689</v>
       </c>
       <c r="F67">
-        <v>0.02260939027250208</v>
+        <v>0.02151005718077093</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2668,7 +2668,7 @@
         <v>1.714803278688525</v>
       </c>
       <c r="F68">
-        <v>0.03857011846866305</v>
+        <v>0.04103964364642074</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2702,7 +2702,7 @@
         <v>45.45065573770492</v>
       </c>
       <c r="F69">
-        <v>1.866964782772334</v>
+        <v>1.982492318657226</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>3.111934426229508</v>
       </c>
       <c r="F70">
-        <v>0.1076648207580059</v>
+        <v>0.1161255401134119</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2770,7 +2770,7 @@
         <v>71.79054098360656</v>
       </c>
       <c r="F71">
-        <v>1.45366148709213</v>
+        <v>1.484468733961409</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2804,7 +2804,7 @@
         <v>13.48934426229508</v>
       </c>
       <c r="F72">
-        <v>0.4295476673793013</v>
+        <v>0.5161560496075248</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2838,7 +2838,7 @@
         <v>0.03201639344262295</v>
       </c>
       <c r="F73">
-        <v>0.005905013841927007</v>
+        <v>0.009150005253267531</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Decreasing</t>
+          <t>Uncertain</t>
         </is>
       </c>
     </row>
@@ -2872,7 +2872,7 @@
         <v>0.1072950819672131</v>
       </c>
       <c r="F74">
-        <v>0.04521454943316253</v>
+        <v>0.04509230550133669</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2906,7 +2906,7 @@
         <v>5.772114754098361</v>
       </c>
       <c r="F75">
-        <v>0.3856308431693886</v>
+        <v>0.4781582164480851</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2940,7 +2940,7 @@
         <v>3.197508196721312</v>
       </c>
       <c r="F76">
-        <v>0.2942235922770435</v>
+        <v>0.3626490045491643</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update spreadsheet with new death 31/61 day averages
</commit_message>
<xml_diff>
--- a/Output/Difference in moving averages16Oct.xlsx
+++ b/Output/Difference in moving averages16Oct.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +402,17 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>Status of cases</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>31-day average of new deaths per million on end_date</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>61-day average of new deaths per million on end_date</t>
         </is>
       </c>
     </row>
@@ -439,6 +449,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I2">
+        <v>0.0455483870967742</v>
+      </c>
+      <c r="J2">
+        <v>0.04672131147540984</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -473,6 +489,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I3">
+        <v>0.1588387096774194</v>
+      </c>
+      <c r="J3">
+        <v>0.1779016393442623</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -507,6 +529,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I4">
+        <v>0.09125806451612903</v>
+      </c>
+      <c r="J4">
+        <v>0.07027868852459017</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -541,6 +569,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I5">
+        <v>0.1663548387096774</v>
+      </c>
+      <c r="J5">
+        <v>0.1973934426229508</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -575,6 +609,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I6">
+        <v>0.002645161290322581</v>
+      </c>
+      <c r="J6">
+        <v>0.002688524590163935</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -609,6 +649,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -643,6 +689,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I8">
+        <v>2.799451612903226</v>
+      </c>
+      <c r="J8">
+        <v>6.184934426229509</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -677,6 +729,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I9">
+        <v>0.01393548387096774</v>
+      </c>
+      <c r="J9">
+        <v>0.008655737704918034</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -711,6 +769,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -745,6 +809,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -779,6 +849,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I12">
+        <v>0.009709677419354839</v>
+      </c>
+      <c r="J12">
+        <v>0.01357377049180328</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -813,6 +889,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I13">
+        <v>1.972806451612903</v>
+      </c>
+      <c r="J13">
+        <v>1.326983606557377</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -847,6 +929,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0.003393442622950819</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -881,6 +969,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I15">
+        <v>0.02164516129032258</v>
+      </c>
+      <c r="J15">
+        <v>0.016</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -915,6 +1009,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -949,6 +1049,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I17">
+        <v>0.02335483870967742</v>
+      </c>
+      <c r="J17">
+        <v>0.09504918032786885</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -983,6 +1089,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I18">
+        <v>0.001225806451612903</v>
+      </c>
+      <c r="J18">
+        <v>0.008098360655737704</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1017,6 +1129,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I19">
+        <v>0.005709677419354839</v>
+      </c>
+      <c r="J19">
+        <v>0.007409836065573771</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1051,6 +1169,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0.03318032786885246</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1085,6 +1209,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I21">
+        <v>0.1345161290322581</v>
+      </c>
+      <c r="J21">
+        <v>0.151672131147541</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1119,6 +1249,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I22">
+        <v>0.5968709677419355</v>
+      </c>
+      <c r="J22">
+        <v>0.7582786885245901</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1153,6 +1289,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1187,6 +1329,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I24">
+        <v>0.08503225806451613</v>
+      </c>
+      <c r="J24">
+        <v>0.1163606557377049</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1221,6 +1369,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I25">
+        <v>0.2003225806451613</v>
+      </c>
+      <c r="J25">
+        <v>0.4341803278688525</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1255,6 +1409,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I26">
+        <v>0.01654838709677419</v>
+      </c>
+      <c r="J26">
+        <v>0.04162295081967214</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1289,6 +1449,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I27">
+        <v>0.01716129032258065</v>
+      </c>
+      <c r="J27">
+        <v>0.02491803278688524</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1323,6 +1489,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I28">
+        <v>0.01638709677419355</v>
+      </c>
+      <c r="J28">
+        <v>0.05831147540983606</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1357,6 +1529,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I29">
+        <v>0.03393548387096774</v>
+      </c>
+      <c r="J29">
+        <v>0.05031147540983606</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1391,6 +1569,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I30">
+        <v>1.51441935483871</v>
+      </c>
+      <c r="J30">
+        <v>1.630327868852459</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1425,6 +1609,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I31">
+        <v>0.7336451612903225</v>
+      </c>
+      <c r="J31">
+        <v>0.738655737704918</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1459,6 +1649,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I32">
+        <v>0.109741935483871</v>
+      </c>
+      <c r="J32">
+        <v>0.1015245901639344</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1493,6 +1689,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I33">
+        <v>0.197741935483871</v>
+      </c>
+      <c r="J33">
+        <v>-0.9850163934426229</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1527,6 +1729,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1561,6 +1769,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I35">
+        <v>0.1355806451612903</v>
+      </c>
+      <c r="J35">
+        <v>0.1301311475409836</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1595,6 +1809,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1629,6 +1849,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I37">
+        <v>0.02787096774193548</v>
+      </c>
+      <c r="J37">
+        <v>0.04190163934426229</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1663,6 +1889,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I38">
+        <v>0.005032258064516129</v>
+      </c>
+      <c r="J38">
+        <v>0.02052459016393442</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1697,6 +1929,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I39">
+        <v>0.00632258064516129</v>
+      </c>
+      <c r="J39">
+        <v>0.005622950819672131</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1731,6 +1969,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I40">
+        <v>0.01387096774193548</v>
+      </c>
+      <c r="J40">
+        <v>0.02114754098360656</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1765,6 +2009,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I41">
+        <v>3.198612903225806</v>
+      </c>
+      <c r="J41">
+        <v>2.580508196721312</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1799,6 +2049,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1833,6 +2089,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I43">
+        <v>1.012129032258065</v>
+      </c>
+      <c r="J43">
+        <v>0.9504918032786885</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1867,6 +2129,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I44">
+        <v>0.0392258064516129</v>
+      </c>
+      <c r="J44">
+        <v>0.02832786885245902</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1901,6 +2169,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I45">
+        <v>0.4345806451612903</v>
+      </c>
+      <c r="J45">
+        <v>0.228672131147541</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1935,6 +2209,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I46">
+        <v>0.3698064516129032</v>
+      </c>
+      <c r="J46">
+        <v>0.3331475409836066</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1969,6 +2249,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I47">
+        <v>0.04870967741935484</v>
+      </c>
+      <c r="J47">
+        <v>0.06436065573770491</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2003,6 +2289,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2037,6 +2329,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I49">
+        <v>0.005290322580645161</v>
+      </c>
+      <c r="J49">
+        <v>0.01139344262295082</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2071,6 +2369,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I50">
+        <v>0.03390322580645162</v>
+      </c>
+      <c r="J50">
+        <v>0.03367213114754098</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2105,6 +2409,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I51">
+        <v>1.378322580645161</v>
+      </c>
+      <c r="J51">
+        <v>1.13744262295082</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2139,6 +2449,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I52">
+        <v>0.003612903225806452</v>
+      </c>
+      <c r="J52">
+        <v>0.007344262295081967</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2173,6 +2489,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I53">
+        <v>0.5496451612903226</v>
+      </c>
+      <c r="J53">
+        <v>0.5830163934426229</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2207,6 +2529,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I54">
+        <v>0.02732258064516129</v>
+      </c>
+      <c r="J54">
+        <v>0.03155737704918032</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2241,6 +2569,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2275,6 +2609,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I56">
+        <v>0.03670967741935484</v>
+      </c>
+      <c r="J56">
+        <v>0.06363934426229508</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2309,6 +2649,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I57">
+        <v>0.004032258064516129</v>
+      </c>
+      <c r="J57">
+        <v>0.00819672131147541</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2340,6 +2686,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2374,6 +2726,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I59">
+        <v>0.002032258064516129</v>
+      </c>
+      <c r="J59">
+        <v>0.00619672131147541</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2408,6 +2766,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I60">
+        <v>0.01725806451612903</v>
+      </c>
+      <c r="J60">
+        <v>0.01168852459016393</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2442,6 +2806,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0.001540983606557377</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2476,6 +2846,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0.01419672131147541</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2510,6 +2886,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I63">
+        <v>0.3892903225806452</v>
+      </c>
+      <c r="J63">
+        <v>0.6500327868852459</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2544,6 +2926,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I64">
+        <v>0.1490645161290323</v>
+      </c>
+      <c r="J64">
+        <v>0.1665737704918033</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2578,6 +2966,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I65">
+        <v>0.02709677419354839</v>
+      </c>
+      <c r="J65">
+        <v>0.02754098360655738</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2612,6 +3006,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2646,6 +3046,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2680,6 +3086,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I68">
+        <v>0.04290322580645161</v>
+      </c>
+      <c r="J68">
+        <v>0.04757377049180328</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2714,6 +3126,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I69">
+        <v>1.078161290322581</v>
+      </c>
+      <c r="J69">
+        <v>0.6352950819672131</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2748,6 +3166,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I70">
+        <v>0.029</v>
+      </c>
+      <c r="J70">
+        <v>0.02985245901639344</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2782,6 +3206,12 @@
           <t>Increasing</t>
         </is>
       </c>
+      <c r="I71">
+        <v>1.54241935483871</v>
+      </c>
+      <c r="J71">
+        <v>1.221295081967213</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2816,6 +3246,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I72">
+        <v>0.1148064516129032</v>
+      </c>
+      <c r="J72">
+        <v>0.1425245901639344</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2850,6 +3286,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0.002180327868852459</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2884,6 +3326,12 @@
           <t>Uncertain</t>
         </is>
       </c>
+      <c r="I74">
+        <v>0.01532258064516129</v>
+      </c>
+      <c r="J74">
+        <v>0.03757377049180328</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2918,6 +3366,12 @@
           <t>Decreasing</t>
         </is>
       </c>
+      <c r="I75">
+        <v>0.0455483870967742</v>
+      </c>
+      <c r="J75">
+        <v>0.07662295081967213</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2951,6 +3405,12 @@
         <is>
           <t>Decreasing</t>
         </is>
+      </c>
+      <c r="I76">
+        <v>0.01512903225806452</v>
+      </c>
+      <c r="J76">
+        <v>0.1113934426229508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>